<commit_message>
creation de contrat fini
</commit_message>
<xml_diff>
--- a/rapport journalier/Rapport journalier - Richard (2).xlsx
+++ b/rapport journalier/Rapport journalier - Richard (2).xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="54">
   <si>
     <t xml:space="preserve">DATE : 22/7/2020</t>
   </si>
@@ -176,6 +176,12 @@
   </si>
   <si>
     <t xml:space="preserve">creation de contrat conexion a la api pour la creation de contrat </t>
+  </si>
+  <si>
+    <t xml:space="preserve">DATE : 24/08/2020</t>
+  </si>
+  <si>
+    <t xml:space="preserve">creation de page paiment </t>
   </si>
 </sst>
 </file>
@@ -511,10 +517,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="B3:J223"/>
+  <dimension ref="B3:J233"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A188" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C216" activeCellId="0" sqref="C216"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A200" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C226" activeCellId="0" sqref="C226"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2124,6 +2130,78 @@
       <c r="H223" s="14"/>
       <c r="I223" s="14"/>
       <c r="J223" s="15"/>
+    </row>
+    <row r="225" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B225" s="16" t="s">
+        <v>52</v>
+      </c>
+      <c r="C225" s="17"/>
+      <c r="D225" s="17"/>
+      <c r="E225" s="18" t="s">
+        <v>1</v>
+      </c>
+      <c r="F225" s="17"/>
+      <c r="G225" s="17"/>
+      <c r="H225" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="I225" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="J225" s="19"/>
+    </row>
+    <row r="226" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B226" s="20" t="s">
+        <v>4</v>
+      </c>
+      <c r="C226" s="0" t="s">
+        <v>53</v>
+      </c>
+      <c r="J226" s="8"/>
+    </row>
+    <row r="227" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B227" s="9"/>
+      <c r="J227" s="8"/>
+    </row>
+    <row r="228" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B228" s="9"/>
+      <c r="J228" s="8"/>
+    </row>
+    <row r="229" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B229" s="21" t="s">
+        <v>7</v>
+      </c>
+      <c r="C229" s="11"/>
+      <c r="D229" s="11"/>
+      <c r="E229" s="11"/>
+      <c r="F229" s="11"/>
+      <c r="G229" s="11"/>
+      <c r="H229" s="11"/>
+      <c r="I229" s="11"/>
+      <c r="J229" s="22"/>
+    </row>
+    <row r="230" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B230" s="9"/>
+      <c r="J230" s="8"/>
+    </row>
+    <row r="231" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B231" s="9"/>
+      <c r="J231" s="8"/>
+    </row>
+    <row r="232" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B232" s="9"/>
+      <c r="J232" s="8"/>
+    </row>
+    <row r="233" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B233" s="13"/>
+      <c r="C233" s="14"/>
+      <c r="D233" s="14"/>
+      <c r="E233" s="14"/>
+      <c r="F233" s="14"/>
+      <c r="G233" s="14"/>
+      <c r="H233" s="14"/>
+      <c r="I233" s="14"/>
+      <c r="J233" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>